<commit_message>
fixed NordLink case, now it works:))
</commit_message>
<xml_diff>
--- a/inertia_sim/N45_case_data_NordLink/dataframes_transparency.xlsx
+++ b/inertia_sim/N45_case_data_NordLink/dataframes_transparency.xlsx
@@ -522,7 +522,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="2">
-        <v>1534</v>
+        <v>8425</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
@@ -530,7 +530,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="2">
-        <v>5234</v>
+        <v>1534</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
@@ -538,7 +538,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="2">
-        <v>2473</v>
+        <v>5234</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
@@ -546,7 +546,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="2">
-        <v>4410</v>
+        <v>2473</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
@@ -554,7 +554,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="2">
-        <v>2693</v>
+        <v>4410</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
@@ -562,7 +562,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="2">
-        <v>3428</v>
+        <v>2693</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
@@ -570,7 +570,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="2">
-        <v>6813</v>
+        <v>3428</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
@@ -578,7 +578,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="2">
-        <v>10111</v>
+        <v>6813</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
@@ -586,7 +586,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="2">
-        <v>2275</v>
+        <v>10111</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
@@ -594,7 +594,7 @@
         <v>25</v>
       </c>
       <c r="B11" s="2">
-        <v>8425</v>
+        <v>2275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>